<commit_message>
Modified testCreateNewAccountWithInvalidData() in TestSell.java
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AmazonTestData.xlsx
+++ b/src/test/resources/TestData/AmazonTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Amazon\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDD4571-D453-4FE2-83D5-60A05AFE28CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E16CF3-01FA-4C3D-80B5-E67581FB451F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{432C8C31-A114-49C0-A38C-A2D746B4FAEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{432C8C31-A114-49C0-A38C-A2D746B4FAEE}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSell" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Expected Result</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Re-Enter Password</t>
+  </si>
+  <si>
+    <t>You indicated you're a new customer, but an account already exists with the email address</t>
   </si>
 </sst>
 </file>
@@ -457,15 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0B423D-1D02-4C4A-ADFB-75148AF5747C}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="73.54296875" customWidth="1"/>
+    <col min="1" max="1" width="100.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -491,6 +494,11 @@
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4C4906-B543-477D-8256-FCEA3EEA2460}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>